<commit_message>
got rid of duplicate entires in BrewBit workbook page
</commit_message>
<xml_diff>
--- a/BrewBitBOMs.xlsx
+++ b/BrewBitBOMs.xlsx
@@ -13,12 +13,15 @@
     <sheet name="CPU Board" sheetId="4" r:id="rId4"/>
     <sheet name="Base Station Board" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BrewBit!$A$1:$J$1</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="447">
   <si>
     <t>Quantity</t>
   </si>
@@ -1344,6 +1347,21 @@
   </si>
   <si>
     <t>S10226 - Hamamatsu Sensor</t>
+  </si>
+  <si>
+    <t>C1, C232, C235, C232, C235</t>
+  </si>
+  <si>
+    <t>R1, R4, R7, R13, R14, R15</t>
+  </si>
+  <si>
+    <t>C3, C9, C10, C11, C12, C13, C21, C291, C21, C291</t>
+  </si>
+  <si>
+    <t>C4, C5, C6, C7, C301, C301</t>
+  </si>
+  <si>
+    <t>Hamamatsu</t>
   </si>
 </sst>
 </file>
@@ -1391,7 +1409,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1414,6 +1432,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC0C0C0"/>
         <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1470,7 +1494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1491,11 +1515,73 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1792,10 +1878,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J92"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1805,7 +1892,7 @@
     <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
     <col min="7" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
@@ -1845,13 +1932,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>28</v>
+        <v>442</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>35</v>
@@ -1907,13 +1994,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>41</v>
+        <v>443</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>47</v>
@@ -1954,14 +2041,14 @@
         <v>48</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5" t="s">
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2027,7 +2114,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>53</v>
@@ -2091,13 +2178,13 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>64</v>
+        <v>444</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>65</v>
@@ -2123,13 +2210,13 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>70</v>
+        <v>445</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>71</v>
@@ -2219,7 +2306,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>27</v>
@@ -2251,7 +2338,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>27</v>
@@ -2347,7 +2434,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>27</v>
@@ -2379,7 +2466,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>27</v>
@@ -2411,16 +2498,16 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>35</v>
+        <v>126</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>34</v>
@@ -2429,16 +2516,16 @@
         <v>11</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>29</v>
+        <v>127</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>30</v>
+        <v>128</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>31</v>
+        <v>129</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>33</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2449,10 +2536,10 @@
         <v>27</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>34</v>
@@ -2461,30 +2548,30 @@
         <v>11</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>34</v>
@@ -2493,30 +2580,30 @@
         <v>11</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>34</v>
@@ -2525,16 +2612,16 @@
         <v>11</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -2542,31 +2629,31 @@
         <v>1</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>27</v>
+        <v>151</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>144</v>
+        <v>32</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>34</v>
+        <v>150</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -2574,10 +2661,10 @@
         <v>1</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>32</v>
@@ -2586,19 +2673,19 @@
         <v>150</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>11</v>
+        <v>158</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -2606,63 +2693,63 @@
         <v>1</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>32</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>158</v>
+        <v>11</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>32</v>
+        <v>168</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>163</v>
+        <v>46</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2673,74 +2760,74 @@
         <v>167</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>46</v>
+        <v>174</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>167</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>174</v>
+        <v>46</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>167</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>46</v>
@@ -2749,16 +2836,16 @@
         <v>11</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2769,10 +2856,10 @@
         <v>167</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>46</v>
@@ -2781,126 +2868,126 @@
         <v>11</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>167</v>
+        <v>202</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>192</v>
+        <v>18</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>193</v>
+        <v>32</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>46</v>
+        <v>201</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>202</v>
+        <v>40</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>18</v>
+        <v>210</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>32</v>
+        <v>211</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>201</v>
+        <v>46</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>207</v>
+        <v>40</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>32</v>
+        <v>217</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>206</v>
+        <v>46</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>211</v>
+        <v>224</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>46</v>
@@ -2909,30 +2996,30 @@
         <v>11</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>214</v>
+        <v>227</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>216</v>
+        <v>229</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>46</v>
@@ -2941,30 +3028,30 @@
         <v>11</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>219</v>
+        <v>232</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>47</v>
+        <v>217</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>46</v>
@@ -2973,16 +3060,16 @@
         <v>11</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>42</v>
+        <v>236</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>43</v>
+        <v>237</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>44</v>
+        <v>238</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>45</v>
+        <v>239</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2993,42 +3080,42 @@
         <v>40</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>223</v>
+        <v>240</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>224</v>
+        <v>242</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>46</v>
+        <v>241</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>225</v>
+        <v>243</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>226</v>
+        <v>244</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>228</v>
+        <v>246</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>46</v>
@@ -3037,30 +3124,30 @@
         <v>11</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>232</v>
+        <v>250</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>233</v>
+        <v>251</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>217</v>
+        <v>47</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>46</v>
@@ -3069,62 +3156,62 @@
         <v>11</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>238</v>
+        <v>256</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>239</v>
+        <v>257</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>240</v>
+        <v>258</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>241</v>
+        <v>46</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>243</v>
+        <v>260</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>244</v>
+        <v>261</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>245</v>
+        <v>262</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>246</v>
+        <v>263</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>248</v>
+        <v>265</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>46</v>
@@ -3133,30 +3220,30 @@
         <v>11</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>251</v>
+        <v>268</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>252</v>
+        <v>269</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>253</v>
+        <v>270</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>47</v>
+        <v>271</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>46</v>
@@ -3165,16 +3252,16 @@
         <v>11</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>254</v>
+        <v>272</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>255</v>
+        <v>273</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>256</v>
+        <v>274</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>257</v>
+        <v>275</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -3185,10 +3272,10 @@
         <v>40</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>258</v>
+        <v>276</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>259</v>
+        <v>277</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>46</v>
@@ -3197,30 +3284,30 @@
         <v>11</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>260</v>
+        <v>278</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>261</v>
+        <v>279</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>262</v>
+        <v>280</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>263</v>
+        <v>281</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>264</v>
+        <v>282</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>265</v>
+        <v>283</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>46</v>
@@ -3229,16 +3316,16 @@
         <v>11</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>266</v>
+        <v>284</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>267</v>
+        <v>285</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>268</v>
+        <v>286</v>
       </c>
       <c r="J45" s="5" t="s">
-        <v>269</v>
+        <v>287</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -3249,10 +3336,10 @@
         <v>40</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>270</v>
+        <v>288</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>271</v>
+        <v>289</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>46</v>
@@ -3261,30 +3348,30 @@
         <v>11</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>272</v>
+        <v>290</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>273</v>
+        <v>291</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>274</v>
+        <v>292</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>275</v>
+        <v>293</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>40</v>
+        <v>295</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>276</v>
+        <v>294</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>277</v>
+        <v>296</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>46</v>
@@ -3293,16 +3380,16 @@
         <v>11</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>279</v>
+        <v>298</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>280</v>
+        <v>299</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>281</v>
+        <v>300</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -3310,31 +3397,31 @@
         <v>1</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>40</v>
+        <v>302</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>282</v>
+        <v>49</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>283</v>
+        <v>32</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>46</v>
+        <v>301</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>284</v>
+        <v>303</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>285</v>
+        <v>304</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>286</v>
+        <v>305</v>
       </c>
       <c r="J48" s="5" t="s">
-        <v>287</v>
+        <v>302</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -3342,63 +3429,63 @@
         <v>1</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>40</v>
+        <v>308</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>288</v>
+        <v>306</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>289</v>
+        <v>32</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>46</v>
+        <v>307</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>290</v>
+        <v>309</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>291</v>
+        <v>310</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>292</v>
+        <v>311</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>295</v>
+        <v>314</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>294</v>
+        <v>312</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>296</v>
+        <v>32</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>46</v>
+        <v>313</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>297</v>
+        <v>315</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>299</v>
+        <v>317</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>300</v>
+        <v>314</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -3406,31 +3493,31 @@
         <v>1</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>302</v>
+        <v>320</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>49</v>
+        <v>318</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>32</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>301</v>
+        <v>319</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>303</v>
+        <v>321</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>304</v>
+        <v>322</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>302</v>
+        <v>320</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -3438,31 +3525,31 @@
         <v>1</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>308</v>
+        <v>326</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>306</v>
+        <v>324</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>32</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>307</v>
+        <v>325</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>309</v>
+        <v>327</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>310</v>
+        <v>328</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>311</v>
+        <v>329</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>308</v>
+        <v>330</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -3470,31 +3557,31 @@
         <v>1</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>314</v>
+        <v>333</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>312</v>
+        <v>331</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>32</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>313</v>
+        <v>332</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>315</v>
+        <v>334</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>316</v>
+        <v>335</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>317</v>
+        <v>336</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>314</v>
+        <v>337</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -3502,31 +3589,31 @@
         <v>1</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>318</v>
+        <v>338</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>32</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>319</v>
+        <v>339</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>321</v>
+        <v>341</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>323</v>
+        <v>343</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>320</v>
+        <v>344</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -3534,31 +3621,31 @@
         <v>1</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>326</v>
+        <v>27</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>324</v>
+        <v>28</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>32</v>
+        <v>346</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>325</v>
+        <v>347</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>327</v>
+        <v>348</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>328</v>
+        <v>349</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>329</v>
+        <v>350</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>330</v>
+        <v>351</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -3566,93 +3653,95 @@
         <v>1</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>333</v>
+        <v>27</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>331</v>
+        <v>352</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>32</v>
+        <v>353</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>332</v>
+        <v>347</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>334</v>
+        <v>354</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>335</v>
+        <v>355</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>336</v>
+        <v>356</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>337</v>
+        <v>357</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>340</v>
+        <v>27</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>338</v>
+        <v>358</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>32</v>
+        <v>359</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>339</v>
+        <v>34</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>341</v>
+        <v>360</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>342</v>
+        <v>361</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>343</v>
+        <v>362</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>344</v>
+        <v>363</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>345</v>
+        <v>27</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D58" s="5"/>
+        <v>365</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>366</v>
+      </c>
       <c r="E58" s="5" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>54</v>
+        <v>367</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>55</v>
+        <v>368</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>56</v>
+        <v>369</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>53</v>
+        <v>370</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
@@ -3660,31 +3749,29 @@
         <v>1</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>27</v>
+        <v>372</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>346</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="D59" s="5"/>
       <c r="E59" s="5" t="s">
-        <v>347</v>
+        <v>373</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>348</v>
+        <v>374</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>349</v>
+        <v>375</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>350</v>
+        <v>376</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>351</v>
+        <v>377</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -3692,191 +3779,187 @@
         <v>1</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>27</v>
+        <v>372</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>353</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="D60" s="5"/>
       <c r="E60" s="5" t="s">
-        <v>347</v>
+        <v>373</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>354</v>
+        <v>378</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>355</v>
+        <v>379</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>356</v>
+        <v>380</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>357</v>
+        <v>381</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>27</v>
+        <v>383</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>359</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D61" s="5"/>
       <c r="E61" s="5" t="s">
-        <v>34</v>
+        <v>384</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>360</v>
+        <v>385</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>361</v>
+        <v>386</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>362</v>
+        <v>387</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>363</v>
+        <v>388</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>88</v>
+        <v>391</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>89</v>
+        <v>392</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>90</v>
+        <v>393</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>91</v>
+        <v>394</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>92</v>
+        <v>395</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>93</v>
+        <v>396</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>364</v>
+        <v>397</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>65</v>
+        <v>398</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>66</v>
+        <v>399</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>67</v>
+        <v>400</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>68</v>
+        <v>401</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>69</v>
+        <v>402</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>94</v>
+        <v>403</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>95</v>
+        <v>404</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>96</v>
+        <v>405</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>97</v>
+        <v>406</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>98</v>
+        <v>407</v>
       </c>
       <c r="J64" s="5" t="s">
-        <v>99</v>
+        <v>408</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>365</v>
+        <v>409</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>366</v>
+        <v>410</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>367</v>
+        <v>411</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>368</v>
+        <v>412</v>
       </c>
       <c r="I65" s="5" t="s">
-        <v>369</v>
+        <v>413</v>
       </c>
       <c r="J65" s="5" t="s">
-        <v>370</v>
+        <v>414</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
@@ -3884,31 +3967,31 @@
         <v>1</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>112</v>
+        <v>415</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>113</v>
+        <v>416</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>114</v>
+        <v>417</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>115</v>
+        <v>418</v>
       </c>
       <c r="I66" s="5" t="s">
-        <v>116</v>
+        <v>419</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>117</v>
+        <v>420</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -3916,820 +3999,101 @@
         <v>1</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>27</v>
+        <v>425</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>119</v>
-      </c>
+        <v>312</v>
+      </c>
+      <c r="D67" s="5"/>
       <c r="E67" s="5" t="s">
-        <v>34</v>
+        <v>313</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>120</v>
+        <v>426</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>121</v>
+        <v>427</v>
       </c>
       <c r="I67" s="5" t="s">
-        <v>122</v>
+        <v>428</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>123</v>
+        <v>429</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>27</v>
+        <v>430</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>35</v>
-      </c>
+        <v>431</v>
+      </c>
+      <c r="D68" s="5"/>
       <c r="E68" s="5" t="s">
-        <v>34</v>
+        <v>430</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>29</v>
+        <v>432</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>30</v>
+        <v>433</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>31</v>
+        <v>434</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>33</v>
+        <v>435</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>27</v>
+        <v>436</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>126</v>
-      </c>
+        <v>338</v>
+      </c>
+      <c r="D69" s="5"/>
       <c r="E69" s="5" t="s">
-        <v>34</v>
+        <v>437</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>127</v>
+        <v>438</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>128</v>
+        <v>439</v>
       </c>
       <c r="I69" s="5" t="s">
-        <v>129</v>
+        <v>440</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="5">
-        <v>1</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G70" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="H70" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="I70" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="J70" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="5">
-        <v>1</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G71" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="H71" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="I71" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="J71" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="5">
-        <v>1</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G72" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="H72" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I72" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="J72" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="5">
-        <v>1</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G73" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="H73" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="I73" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="J73" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="5">
-        <v>1</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G74" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="H74" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="I74" s="5" t="s">
-        <v>376</v>
-      </c>
-      <c r="J74" s="5" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="5">
-        <v>1</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="D75" s="5"/>
-      <c r="E75" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G75" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="H75" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="I75" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="J75" s="5" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="5">
-        <v>1</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G76" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="H76" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="I76" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="J76" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="5">
-        <v>5</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G77" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="H77" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I77" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="J77" s="5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="5">
-        <v>2</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G78" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="H78" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="I78" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="J78" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="5">
-        <v>1</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G79" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="H79" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="I79" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="J79" s="5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="5">
-        <v>1</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G80" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="H80" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="I80" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="J80" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="5">
-        <v>1</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G81" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="H81" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="I81" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="J81" s="5" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="5">
-        <v>2</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>391</v>
-      </c>
-      <c r="D82" s="5" t="s">
-        <v>392</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G82" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="H82" s="5" t="s">
-        <v>394</v>
-      </c>
-      <c r="I82" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="J82" s="5" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="5">
-        <v>1</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>397</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>398</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G83" s="5" t="s">
-        <v>399</v>
-      </c>
-      <c r="H83" s="5" t="s">
-        <v>400</v>
-      </c>
-      <c r="I83" s="5" t="s">
-        <v>401</v>
-      </c>
-      <c r="J83" s="5" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="5">
-        <v>1</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>403</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="E84" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G84" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="H84" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="I84" s="5" t="s">
-        <v>407</v>
-      </c>
-      <c r="J84" s="5" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="5">
-        <v>1</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G85" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="H85" s="5" t="s">
-        <v>412</v>
-      </c>
-      <c r="I85" s="5" t="s">
-        <v>413</v>
-      </c>
-      <c r="J85" s="5" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="5">
-        <v>1</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="D86" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F86" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G86" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="H86" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="I86" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="J86" s="5" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="5">
-        <v>1</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>415</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>416</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G87" s="5" t="s">
-        <v>417</v>
-      </c>
-      <c r="H87" s="5" t="s">
-        <v>418</v>
-      </c>
-      <c r="I87" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="J87" s="5" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="5">
-        <v>1</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="D88" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G88" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="H88" s="5" t="s">
-        <v>421</v>
-      </c>
-      <c r="I88" s="5" t="s">
-        <v>422</v>
-      </c>
-      <c r="J88" s="5" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="5">
-        <v>1</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C89" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G89" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="H89" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="I89" s="5" t="s">
-        <v>424</v>
-      </c>
-      <c r="J89" s="5" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="5">
-        <v>1</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="C90" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G90" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="H90" s="5" t="s">
-        <v>427</v>
-      </c>
-      <c r="I90" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="J90" s="5" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="5">
-        <v>1</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>430</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>431</v>
-      </c>
-      <c r="D91" s="5"/>
-      <c r="E91" s="5" t="s">
-        <v>430</v>
-      </c>
-      <c r="F91" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G91" s="5" t="s">
-        <v>432</v>
-      </c>
-      <c r="H91" s="5" t="s">
-        <v>433</v>
-      </c>
-      <c r="I91" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="J91" s="5" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="5">
-        <v>1</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>436</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="D92" s="5"/>
-      <c r="E92" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="F92" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G92" s="5" t="s">
-        <v>438</v>
-      </c>
-      <c r="H92" s="5" t="s">
-        <v>439</v>
-      </c>
-      <c r="I92" s="5" t="s">
-        <v>440</v>
-      </c>
-      <c r="J92" s="5" t="s">
-        <v>437</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J1"/>
+  <dataConsolidate/>
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L6">
+    <cfRule type="uniqueValues" dxfId="4" priority="2"/>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN101/311-1024-1-ND/302941"/>
     <hyperlink ref="I4" r:id="rId2" display="http://www.digikey.com/product-detail/en/ERJ-2GEJ103X/P10KJDKR-ND/577446"/>
@@ -4741,75 +4105,52 @@
     <hyperlink ref="I7" r:id="rId8" display="http://www.digikey.com/product-detail/en/951104-4620-AR-PR/3M9353DKR-ND/1959790"/>
     <hyperlink ref="H6" r:id="rId9" display="http://www.digikey.com/product-detail/en/70ADJ-2-ML1G/70ADJ-2-ML1GTR-ND/2537935"/>
     <hyperlink ref="H7" r:id="rId10" display="http://www.digikey.com/product-detail/en/951104-4620-AR-PR/3M9353TR-ND/1959081"/>
-    <hyperlink ref="G25" r:id="rId11" display="http://www.digikey.com/product-detail/en/BAT54C-V-GS08/BAT54C-V-GS08GICT-ND/2684798"/>
-    <hyperlink ref="H25" r:id="rId12" display="http://www.digikey.com/product-detail/en/BAT54C-V-GS08/BAT54C-V-GS08GITR-ND/1125418"/>
-    <hyperlink ref="I25" r:id="rId13" display="http://www.digikey.com/product-detail/en/BAT54C-V-GS08/BAT54C-V-GS08GIDKR-ND/2684803"/>
-    <hyperlink ref="G26" r:id="rId14" display="http://www.digikey.com/product-detail/en/AZ23C5V6-V-GS08/AZ23C5V6-V-GS08CT-ND/3104408"/>
-    <hyperlink ref="H26" r:id="rId15" display="http://www.digikey.com/product-detail/en/AZ23C5V6-V-GS08/AZ23C5V6-V-GS08TR-ND/3104165"/>
-    <hyperlink ref="I26" r:id="rId16" display="http://www.digikey.com/product-detail/en/AZ23C5V6-V-GS08/AZ23C5V6-V-GS08DKR-ND/3104547"/>
-    <hyperlink ref="G35" r:id="rId17" display="http://www.digikey.com/product-detail/en/ERJ-2GEJ152X/P1.5KJCT-ND/146913"/>
-    <hyperlink ref="H35" r:id="rId18" display="http://www.digikey.com/product-detail/en/ERJ-2GEJ152X/P1.5KJTR-ND/146914"/>
-    <hyperlink ref="I35" r:id="rId19" display="http://www.digikey.com/product-detail/en/ERJ-2GEJ152X/P1.5KJDKR-ND/577470"/>
-    <hyperlink ref="G36" r:id="rId20" display="http://www.digikey.com/product-detail/en/ERJ-2GEJ101X/P100JCT-ND/146728"/>
-    <hyperlink ref="I36" r:id="rId21" display="http://www.digikey.com/product-detail/en/ERJ-2GEJ101X/P100JDKR-ND/577444"/>
-    <hyperlink ref="G53" r:id="rId22" display="http://www.digikey.com/product-detail/en/CC1110F32RSPR/296-22740-1-ND/1739899"/>
-    <hyperlink ref="H53" r:id="rId23" display="http://www.digikey.com/product-detail/en/CC1110F32RSPR/296-22740-2-ND/1739757"/>
-    <hyperlink ref="I53" r:id="rId24" display="http://www.digikey.com/product-detail/en/CC1110F32RSPR/296-22740-6-ND/1740017"/>
-    <hyperlink ref="G20" r:id="rId25" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN101/311-1024-1-ND/302941"/>
-    <hyperlink ref="H20" r:id="rId26" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN101/311-1024-2-ND/302758"/>
-    <hyperlink ref="I20" r:id="rId27" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN101/311-1024-6-ND/578920"/>
-    <hyperlink ref="J20" r:id="rId28" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN101/311-1024-1-ND/302941"/>
-    <hyperlink ref="G21" r:id="rId29" display="http://www.digikey.com/product-detail/en/C1005C0G1H1R5B/445-4858-1-ND/2093472"/>
-    <hyperlink ref="H21" r:id="rId30" display="http://www.digikey.com/product-detail/en/C1005C0G1H1R5B/445-4858-2-ND/2093126"/>
-    <hyperlink ref="I21" r:id="rId31" display="http://www.digikey.com/product-detail/en/C1005C0G1H1R5B/445-4858-6-ND/2093824"/>
-    <hyperlink ref="J21" r:id="rId32" display="http://www.digikey.com/product-detail/en/C1005C0G1H1R5B/445-4858-1-ND/2093472"/>
-    <hyperlink ref="G22" r:id="rId33" display="http://www.digikey.com/product-detail/en/C1005C0G1H3R3B/445-4871-1-ND/2093485"/>
-    <hyperlink ref="H22" r:id="rId34" display="http://www.digikey.com/product-detail/en/C1005C0G1H3R3B/445-4871-2-ND/2093139"/>
-    <hyperlink ref="I22" r:id="rId35" display="http://www.digikey.com/product-detail/en/C1005C0G1H3R3B/445-4871-6-ND/2093837"/>
-    <hyperlink ref="J22" r:id="rId36" display="http://www.digikey.com/product-detail/en/C1005C0G1H3R3B/445-4871-6-ND/2093837"/>
-    <hyperlink ref="G9" r:id="rId37" display="http://www.digikey.com/product-detail/en/C2012Y5V1A106Z/445-1371-1-ND/567608"/>
-    <hyperlink ref="H9" r:id="rId38" display="http://www.digikey.com/product-detail/en/C2012Y5V1A106Z/445-1371-2-ND/513923"/>
-    <hyperlink ref="I9" r:id="rId39" display="http://www.digikey.com/product-detail/en/C2012Y5V1A106Z/445-1371-6-ND/1725625"/>
-    <hyperlink ref="J9" r:id="rId40" display="http://www.digikey.com/product-detail/en/C2012Y5V1A106Z/445-1371-6-ND/1725625"/>
-    <hyperlink ref="G16" r:id="rId41" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN150/311-1017-1-ND/302934"/>
-    <hyperlink ref="H16" r:id="rId42" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN150/311-1017-2-ND/302751"/>
-    <hyperlink ref="I16" r:id="rId43" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN150/311-1017-6-ND/578924"/>
-    <hyperlink ref="J16" r:id="rId44" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN150/311-1017-6-ND/578924"/>
-    <hyperlink ref="G17" r:id="rId45" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN120/311-1016-1-ND/302933"/>
-    <hyperlink ref="I17" r:id="rId46" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN120/311-1016-6-ND/578922"/>
-    <hyperlink ref="J17" r:id="rId47" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN120/311-1016-6-ND/578922"/>
-    <hyperlink ref="G18" r:id="rId48" display="http://www.digikey.com/product-detail/en/CC0402CRNPO9BN2R2/311-1354-1-ND/2103138"/>
-    <hyperlink ref="H18" r:id="rId49" display="http://www.digikey.com/product-detail/en/CC0402CRNPO9BN2R2/311-1354-2-ND/2103092"/>
-    <hyperlink ref="I18" r:id="rId50" display="http://www.digikey.com/product-detail/en/CC0402CRNPO9BN2R2/311-1354-6-ND/2103184"/>
-    <hyperlink ref="J18" r:id="rId51" display="http://www.digikey.com/product-detail/en/CC0402CRNPO9BN2R2/311-1354-6-ND/2103184"/>
-    <hyperlink ref="H58" r:id="rId52"/>
-    <hyperlink ref="I58" r:id="rId53"/>
-    <hyperlink ref="G59" r:id="rId54"/>
-    <hyperlink ref="G74" r:id="rId55"/>
-    <hyperlink ref="H74" r:id="rId56"/>
-    <hyperlink ref="I74" r:id="rId57"/>
-    <hyperlink ref="G80" r:id="rId58"/>
-    <hyperlink ref="G82" r:id="rId59"/>
-    <hyperlink ref="H82" r:id="rId60"/>
-    <hyperlink ref="G90" r:id="rId61"/>
-    <hyperlink ref="H90" r:id="rId62"/>
-    <hyperlink ref="I90" r:id="rId63"/>
-    <hyperlink ref="G66" r:id="rId64" display="http://www.digikey.com/product-detail/en/CC0402CRNPO9BN2R2/311-1354-1-ND/2103138"/>
-    <hyperlink ref="H66" r:id="rId65" display="http://www.digikey.com/product-detail/en/CC0402CRNPO9BN2R2/311-1354-2-ND/2103092"/>
-    <hyperlink ref="I66" r:id="rId66" display="http://www.digikey.com/product-detail/en/CC0402CRNPO9BN2R2/311-1354-6-ND/2103184"/>
-    <hyperlink ref="J66" r:id="rId67" display="http://www.digikey.com/product-detail/en/CC0402CRNPO9BN2R2/311-1354-6-ND/2103184"/>
-    <hyperlink ref="G68" r:id="rId68" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN101/311-1024-1-ND/302941"/>
-    <hyperlink ref="H68" r:id="rId69" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN101/311-1024-2-ND/302758"/>
-    <hyperlink ref="I68" r:id="rId70" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN101/311-1024-6-ND/578920"/>
-    <hyperlink ref="J68" r:id="rId71" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN101/311-1024-6-ND/578920"/>
-    <hyperlink ref="G69" r:id="rId72" display="http://www.digikey.com/product-detail/en/C1005C0G1H1R5B/445-4858-1-ND/2093472"/>
-    <hyperlink ref="H69" r:id="rId73" display="http://www.digikey.com/product-detail/en/C1005C0G1H1R5B/445-4858-2-ND/2093126"/>
-    <hyperlink ref="I69" r:id="rId74" display="http://www.digikey.com/product-detail/en/C1005C0G1H1R5B/445-4858-6-ND/2093824"/>
-    <hyperlink ref="J69" r:id="rId75" display="http://www.digikey.com/product-detail/en/C1005C0G1H1R5B/445-4858-6-ND/2093824"/>
-    <hyperlink ref="G70" r:id="rId76" display="http://www.digikey.com/product-detail/en/C1005C0G1H3R3B/445-4871-1-ND/2093485"/>
-    <hyperlink ref="H70" r:id="rId77" display="http://www.digikey.com/product-detail/en/C1005C0G1H3R3B/445-4871-2-ND/2093139"/>
-    <hyperlink ref="I70" r:id="rId78" display="http://www.digikey.com/product-detail/en/C1005C0G1H3R3B/445-4871-6-ND/2093837"/>
-    <hyperlink ref="J70" r:id="rId79" display="http://www.digikey.com/product-detail/en/C1005C0G1H3R3B/445-4871-6-ND/2093837"/>
+    <hyperlink ref="G24" r:id="rId11" display="http://www.digikey.com/product-detail/en/BAT54C-V-GS08/BAT54C-V-GS08GICT-ND/2684798"/>
+    <hyperlink ref="H24" r:id="rId12" display="http://www.digikey.com/product-detail/en/BAT54C-V-GS08/BAT54C-V-GS08GITR-ND/1125418"/>
+    <hyperlink ref="I24" r:id="rId13" display="http://www.digikey.com/product-detail/en/BAT54C-V-GS08/BAT54C-V-GS08GIDKR-ND/2684803"/>
+    <hyperlink ref="G25" r:id="rId14" display="http://www.digikey.com/product-detail/en/AZ23C5V6-V-GS08/AZ23C5V6-V-GS08CT-ND/3104408"/>
+    <hyperlink ref="H25" r:id="rId15" display="http://www.digikey.com/product-detail/en/AZ23C5V6-V-GS08/AZ23C5V6-V-GS08TR-ND/3104165"/>
+    <hyperlink ref="I25" r:id="rId16" display="http://www.digikey.com/product-detail/en/AZ23C5V6-V-GS08/AZ23C5V6-V-GS08DKR-ND/3104547"/>
+    <hyperlink ref="G33" r:id="rId17" display="http://www.digikey.com/product-detail/en/ERJ-2GEJ152X/P1.5KJCT-ND/146913"/>
+    <hyperlink ref="H33" r:id="rId18" display="http://www.digikey.com/product-detail/en/ERJ-2GEJ152X/P1.5KJTR-ND/146914"/>
+    <hyperlink ref="I33" r:id="rId19" display="http://www.digikey.com/product-detail/en/ERJ-2GEJ152X/P1.5KJDKR-ND/577470"/>
+    <hyperlink ref="G34" r:id="rId20" display="http://www.digikey.com/product-detail/en/ERJ-2GEJ101X/P100JCT-ND/146728"/>
+    <hyperlink ref="I34" r:id="rId21" display="http://www.digikey.com/product-detail/en/ERJ-2GEJ101X/P100JDKR-ND/577444"/>
+    <hyperlink ref="G50" r:id="rId22" display="http://www.digikey.com/product-detail/en/CC1110F32RSPR/296-22740-1-ND/1739899"/>
+    <hyperlink ref="H50" r:id="rId23" display="http://www.digikey.com/product-detail/en/CC1110F32RSPR/296-22740-2-ND/1739757"/>
+    <hyperlink ref="I50" r:id="rId24" display="http://www.digikey.com/product-detail/en/CC1110F32RSPR/296-22740-6-ND/1740017"/>
+    <hyperlink ref="G20" r:id="rId25" display="http://www.digikey.com/product-detail/en/C1005C0G1H1R5B/445-4858-1-ND/2093472"/>
+    <hyperlink ref="H20" r:id="rId26" display="http://www.digikey.com/product-detail/en/C1005C0G1H1R5B/445-4858-2-ND/2093126"/>
+    <hyperlink ref="I20" r:id="rId27" display="http://www.digikey.com/product-detail/en/C1005C0G1H1R5B/445-4858-6-ND/2093824"/>
+    <hyperlink ref="J20" r:id="rId28" display="http://www.digikey.com/product-detail/en/C1005C0G1H1R5B/445-4858-1-ND/2093472"/>
+    <hyperlink ref="G21" r:id="rId29" display="http://www.digikey.com/product-detail/en/C1005C0G1H3R3B/445-4871-1-ND/2093485"/>
+    <hyperlink ref="H21" r:id="rId30" display="http://www.digikey.com/product-detail/en/C1005C0G1H3R3B/445-4871-2-ND/2093139"/>
+    <hyperlink ref="I21" r:id="rId31" display="http://www.digikey.com/product-detail/en/C1005C0G1H3R3B/445-4871-6-ND/2093837"/>
+    <hyperlink ref="J21" r:id="rId32" display="http://www.digikey.com/product-detail/en/C1005C0G1H3R3B/445-4871-6-ND/2093837"/>
+    <hyperlink ref="G9" r:id="rId33" display="http://www.digikey.com/product-detail/en/C2012Y5V1A106Z/445-1371-1-ND/567608"/>
+    <hyperlink ref="H9" r:id="rId34" display="http://www.digikey.com/product-detail/en/C2012Y5V1A106Z/445-1371-2-ND/513923"/>
+    <hyperlink ref="I9" r:id="rId35" display="http://www.digikey.com/product-detail/en/C2012Y5V1A106Z/445-1371-6-ND/1725625"/>
+    <hyperlink ref="J9" r:id="rId36" display="http://www.digikey.com/product-detail/en/C2012Y5V1A106Z/445-1371-6-ND/1725625"/>
+    <hyperlink ref="G16" r:id="rId37" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN150/311-1017-1-ND/302934"/>
+    <hyperlink ref="H16" r:id="rId38" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN150/311-1017-2-ND/302751"/>
+    <hyperlink ref="I16" r:id="rId39" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN150/311-1017-6-ND/578924"/>
+    <hyperlink ref="J16" r:id="rId40" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN150/311-1017-6-ND/578924"/>
+    <hyperlink ref="G17" r:id="rId41" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN120/311-1016-1-ND/302933"/>
+    <hyperlink ref="I17" r:id="rId42" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN120/311-1016-6-ND/578922"/>
+    <hyperlink ref="J17" r:id="rId43" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN120/311-1016-6-ND/578922"/>
+    <hyperlink ref="G18" r:id="rId44" display="http://www.digikey.com/product-detail/en/CC0402CRNPO9BN2R2/311-1354-1-ND/2103138"/>
+    <hyperlink ref="H18" r:id="rId45" display="http://www.digikey.com/product-detail/en/CC0402CRNPO9BN2R2/311-1354-2-ND/2103092"/>
+    <hyperlink ref="I18" r:id="rId46" display="http://www.digikey.com/product-detail/en/CC0402CRNPO9BN2R2/311-1354-6-ND/2103184"/>
+    <hyperlink ref="J18" r:id="rId47" display="http://www.digikey.com/product-detail/en/CC0402CRNPO9BN2R2/311-1354-6-ND/2103184"/>
+    <hyperlink ref="G55" r:id="rId48"/>
+    <hyperlink ref="G59" r:id="rId49"/>
+    <hyperlink ref="H59" r:id="rId50"/>
+    <hyperlink ref="I59" r:id="rId51"/>
+    <hyperlink ref="G62" r:id="rId52"/>
+    <hyperlink ref="H62" r:id="rId53"/>
+    <hyperlink ref="G67" r:id="rId54"/>
+    <hyperlink ref="H67" r:id="rId55"/>
+    <hyperlink ref="I67" r:id="rId56"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4820,7 +4161,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fixed some mistakes and removed old unused parts
</commit_message>
<xml_diff>
--- a/BrewBitBOMs.xlsx
+++ b/BrewBitBOMs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="14115"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="27795" windowHeight="14115" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BrewBit" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="449">
   <si>
     <t>Quantity</t>
   </si>
@@ -1362,6 +1362,12 @@
   </si>
   <si>
     <t>Hamamatsu</t>
+  </si>
+  <si>
+    <t>Manufacturer Part Number</t>
+  </si>
+  <si>
+    <t>CC1111F32RSPR</t>
   </si>
 </sst>
 </file>
@@ -1520,7 +1526,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1538,36 +1544,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1880,22 +1856,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="D38" sqref="A38:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1927,7 +1903,7 @@
         <v>25</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>7</v>
+        <v>447</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -4021,7 +3997,7 @@
         <v>428</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>429</v>
+        <v>448</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
@@ -4088,11 +4064,11 @@
   <autoFilter ref="A1:J1"/>
   <dataConsolidate/>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6">
-    <cfRule type="uniqueValues" dxfId="4" priority="2"/>
+    <cfRule type="uniqueValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" display="http://www.digikey.com/product-detail/en/CC0402JRNPO9BN101/311-1024-1-ND/302941"/>
@@ -4472,8 +4448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J52"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>